<commit_message>
start making logic paper on git
</commit_message>
<xml_diff>
--- a/LogicPaper.xlsx
+++ b/LogicPaper.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24315" windowHeight="10395" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24315" windowHeight="10395" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="DEFOX" sheetId="2" r:id="rId1"/>
     <sheet name="cyborg" sheetId="1" r:id="rId2"/>
     <sheet name="math" sheetId="3" r:id="rId3"/>
     <sheet name="mirror" sheetId="4" r:id="rId4"/>
+    <sheet name="nm" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="M_U" localSheetId="3">mirror!$E$123:$F$124</definedName>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="127">
   <si>
     <t>Structures</t>
     <phoneticPr fontId="4"/>
@@ -450,6 +451,98 @@
     <t>hence U is a 2 x 2 matrix, it must have another eigen value and vector</t>
     <phoneticPr fontId="3"/>
   </si>
+  <si>
+    <t>Newton Method</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Polynomials</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>some origami Axioms require to solve</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Quadratic Equation</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Cubic Equation</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Axiom 3</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Axiom 5</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Axiom 7</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Axiom 6</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>+</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>*</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>/</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>other than root operations:</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>, while DEFOX implements only 4 arithmetic operations:</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>, which leads numbers to out of the Field (~ rational numbers)</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Approximation</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>DEFOX tries to approximate these roots by solving the equation by Newton Method</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Newton Method is one of the fastest solver algorithm</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>But it is also known as "generally unstable method" wrt the initial value</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>using a reccurence relaion</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Here, we focusing on solving Quadratic equations;</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>, which the unstability can be managed eazily shown as follows</t>
+    <phoneticPr fontId="3"/>
+  </si>
 </sst>
 </file>
 
@@ -689,7 +782,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -751,6 +844,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -897,16 +993,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.69721881222178816</c:v>
+                  <c:v>1.5613777095521697</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.4663021827176905</c:v>
+                  <c:v>3.8835988679248867E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.99386746875143706</c:v>
+                  <c:v>7.9846708039983652</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.7063501136337305</c:v>
+                  <c:v>2.7567454201469377</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -918,16 +1014,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.50172406692161164</c:v>
+                  <c:v>9.1756971777813465</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.5511220008408637</c:v>
+                  <c:v>3.9027212035321259</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.5593805909316583</c:v>
+                  <c:v>2.0550840591688893</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8643616804719878</c:v>
+                  <c:v>0.44260465163959428</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -979,16 +1075,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-4.8335661631773537</c:v>
+                  <c:v>3.2514835319954853</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3.1214874903537249</c:v>
+                  <c:v>-1.3842617214393491</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.7787224760439893</c:v>
+                  <c:v>-5.3828271283174089</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.367990818564337</c:v>
+                  <c:v>-5.4669882520671322</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1000,16 +1096,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4.6498127984709674</c:v>
+                  <c:v>7.9081178109488599</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.241964255644424</c:v>
+                  <c:v>4.9700444861210737</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.4707393354622438</c:v>
+                  <c:v>12.08070750840572</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.920117379620537</c:v>
+                  <c:v>6.6104049058001468</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1094,11 +1190,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1428086144"/>
-        <c:axId val="-1428091040"/>
+        <c:axId val="2023158704"/>
+        <c:axId val="2023159248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1428086144"/>
+        <c:axId val="2023158704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1155,12 +1251,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1428091040"/>
+        <c:crossAx val="2023159248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1428091040"/>
+        <c:axId val="2023159248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1217,7 +1313,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1428086144"/>
+        <c:crossAx val="2023158704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2863,13 +2959,7 @@
                       <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>=</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>0</m:t>
+                      <m:t>=0</m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -3342,19 +3432,7 @@
                       <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>∗</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>1</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>=</m:t>
+                      <m:t>∗1=</m:t>
                     </m:r>
                     <m:r>
                       <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
@@ -4168,13 +4246,7 @@
                       <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>−</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>2</m:t>
+                      <m:t>−2</m:t>
                     </m:r>
                     <m:r>
                       <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
@@ -4198,13 +4270,7 @@
                       <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>=</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>0</m:t>
+                      <m:t>=0</m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -5167,8 +5233,8 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2052228" cy="229615"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="テキスト ボックス 1"/>
@@ -5361,7 +5427,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="テキスト ボックス 1"/>
@@ -5420,8 +5486,8 @@
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1256049" cy="223074"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="テキスト ボックス 3"/>
@@ -5572,7 +5638,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="テキスト ボックス 3"/>
@@ -5631,8 +5697,8 @@
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2197974" cy="290464"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="テキスト ボックス 4"/>
@@ -5844,7 +5910,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="テキスト ボックス 4"/>
@@ -5903,8 +5969,8 @@
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2808589" cy="433837"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="テキスト ボックス 5"/>
@@ -6076,13 +6142,7 @@
                                 <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 </a:rPr>
-                                <m:t>−</m:t>
-                              </m:r>
-                              <m:r>
-                                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                </a:rPr>
-                                <m:t>1</m:t>
+                                <m:t>−1</m:t>
                               </m:r>
                             </m:e>
                           </m:mr>
@@ -6238,7 +6298,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="テキスト ボックス 5"/>
@@ -6297,8 +6357,8 @@
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="775533" cy="219163"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="テキスト ボックス 6"/>
@@ -6372,13 +6432,7 @@
                       <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>=</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>0</m:t>
+                      <m:t>=0</m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -6388,7 +6442,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="テキスト ボックス 6"/>
@@ -6447,8 +6501,8 @@
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2028569" cy="971035"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="テキスト ボックス 7"/>
@@ -6890,7 +6944,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="テキスト ボックス 7"/>
@@ -7022,8 +7076,8 @@
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1875450" cy="219163"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="テキスト ボックス 8"/>
@@ -7180,7 +7234,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="テキスト ボックス 8"/>
@@ -7239,8 +7293,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1789464" cy="559577"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="テキスト ボックス 9"/>
@@ -7687,7 +7741,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="テキスト ボックス 9"/>
@@ -7819,8 +7873,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1082861" cy="445828"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="テキスト ボックス 10"/>
@@ -7973,7 +8027,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="テキスト ボックス 10"/>
@@ -8032,8 +8086,8 @@
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1087734" cy="445828"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="テキスト ボックス 11"/>
@@ -8186,7 +8240,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="テキスト ボックス 11"/>
@@ -8245,8 +8299,8 @@
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1803571" cy="1076064"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="テキスト ボックス 12"/>
@@ -8438,13 +8492,7 @@
                       <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>−</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>2</m:t>
+                      <m:t>−2</m:t>
                     </m:r>
                     <m:r>
                       <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
@@ -8502,13 +8550,7 @@
                       <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>−</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>2</m:t>
+                      <m:t>−2</m:t>
                     </m:r>
                     <m:f>
                       <m:fPr>
@@ -8627,7 +8669,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="テキスト ボックス 12"/>
@@ -8720,8 +8762,8 @@
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2885982" cy="433580"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="テキスト ボックス 13"/>
@@ -9021,7 +9063,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="テキスト ボックス 13"/>
@@ -9080,8 +9122,8 @@
       <xdr:rowOff>228600</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2596608" cy="484043"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="テキスト ボックス 14"/>
@@ -9149,13 +9191,7 @@
                           <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
-                          <m:t>−</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>2</m:t>
+                          <m:t>−2</m:t>
                         </m:r>
                         <m:f>
                           <m:fPr>
@@ -9271,13 +9307,7 @@
                       <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>+</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>2</m:t>
+                      <m:t>+2</m:t>
                     </m:r>
                     <m:f>
                       <m:fPr>
@@ -9390,7 +9420,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="テキスト ボックス 14"/>
@@ -9449,8 +9479,8 @@
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1822422" cy="891654"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="18" name="テキスト ボックス 17"/>
@@ -9547,23 +9577,7 @@
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
-                      <m:t>−</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                        <a:ln>
-                          <a:noFill/>
-                        </a:ln>
-                        <a:solidFill>
-                          <a:prstClr val="black"/>
-                        </a:solidFill>
-                        <a:effectLst/>
-                        <a:uLnTx/>
-                        <a:uFillTx/>
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:rPr>
-                      <m:t>2</m:t>
+                      <m:t>−2</m:t>
                     </m:r>
                     <m:f>
                       <m:fPr>
@@ -10069,7 +10083,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="18" name="テキスト ボックス 17"/>
@@ -10207,8 +10221,8 @@
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1147429" cy="229615"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="17" name="テキスト ボックス 16"/>
@@ -10244,6 +10258,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -10368,7 +10383,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="17" name="テキスト ボックス 16"/>
@@ -10426,8 +10441,8 @@
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1956561" cy="665503"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="20" name="テキスト ボックス 19"/>
@@ -10463,6 +10478,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -10541,13 +10557,7 @@
                       <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>−</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>2</m:t>
+                      <m:t>−2</m:t>
                     </m:r>
                     <m:f>
                       <m:fPr>
@@ -10811,7 +10821,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="20" name="テキスト ボックス 19"/>
@@ -10930,8 +10940,8 @@
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="271677" cy="219163"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="21" name="テキスト ボックス 20"/>
@@ -10967,6 +10977,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -11000,7 +11011,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="21" name="テキスト ボックス 20"/>
@@ -11058,8 +11069,8 @@
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2929392" cy="1575624"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="22" name="テキスト ボックス 21"/>
@@ -11095,6 +11106,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -11180,7 +11192,7 @@
                     <m:f>
                       <m:fPr>
                         <m:ctrlPr>
-                          <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="0">
+                          <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -11298,19 +11310,7 @@
                       <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>=</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>2</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>−</m:t>
+                      <m:t>=2−</m:t>
                     </m:r>
                     <m:f>
                       <m:fPr>
@@ -11808,37 +11808,7 @@
                       <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>=</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>2</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>−</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>2</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>−</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>0</m:t>
+                      <m:t>=2−2−0</m:t>
                     </m:r>
                   </m:oMath>
                   <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
@@ -11846,13 +11816,7 @@
                       <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>=</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>0</m:t>
+                      <m:t>=0</m:t>
                     </m:r>
                   </m:oMath>
                   <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
@@ -11860,19 +11824,7 @@
                       <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>⇒</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>0</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>−</m:t>
+                      <m:t>⇒0−</m:t>
                     </m:r>
                     <m:d>
                       <m:dPr>
@@ -11887,13 +11839,7 @@
                           <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
-                          <m:t>−</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>1</m:t>
+                          <m:t>−1</m:t>
                         </m:r>
                       </m:e>
                     </m:d>
@@ -11901,13 +11847,7 @@
                       <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>=</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>1</m:t>
+                      <m:t>=1</m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -11917,7 +11857,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="22" name="テキスト ボックス 21"/>
@@ -12071,8 +12011,8 @@
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1470403" cy="452175"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="23" name="テキスト ボックス 22"/>
@@ -12108,6 +12048,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -12478,7 +12419,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="23" name="テキスト ボックス 22"/>
@@ -12552,8 +12493,8 @@
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1649682" cy="681469"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="24" name="テキスト ボックス 23"/>
@@ -12589,6 +12530,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -12879,7 +12821,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="24" name="テキスト ボックス 23"/>
@@ -12963,8 +12905,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1589794" cy="229615"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="25" name="テキスト ボックス 24"/>
@@ -13000,6 +12942,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -13162,7 +13105,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="25" name="テキスト ボックス 24"/>
@@ -13220,8 +13163,8 @@
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1602297" cy="229615"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="26" name="テキスト ボックス 25"/>
@@ -13257,6 +13200,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -13419,7 +13363,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="26" name="テキスト ボックス 25"/>
@@ -13477,8 +13421,8 @@
       <xdr:rowOff>209550</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2894126" cy="731419"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="27" name="テキスト ボックス 26"/>
@@ -13514,6 +13458,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -14259,7 +14204,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="27" name="テキスト ボックス 26"/>
@@ -14399,8 +14344,8 @@
       <xdr:rowOff>209550</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1599797" cy="459228"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="28" name="テキスト ボックス 27"/>
@@ -14436,6 +14381,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -14716,7 +14662,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="28" name="テキスト ボックス 27"/>
@@ -14770,6 +14716,452 @@
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>|𝑛′〉≔𝑈 ̂_2 |𝑛_1^′ 〉+|𝑛_2^′ 〉</a:t>
+              </a:r>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>271462</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="395288" cy="279115"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="テキスト ボックス 1"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1643062" y="4443412"/>
+              <a:ext cx="395288" cy="279115"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:rad>
+                      <m:radPr>
+                        <m:degHide m:val="on"/>
+                        <m:ctrlPr>
+                          <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:radPr>
+                      <m:deg/>
+                      <m:e/>
+                    </m:rad>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="テキスト ボックス 1"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1643062" y="4443412"/>
+              <a:ext cx="395288" cy="279115"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>√</a:t>
+              </a:r>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="395288" cy="279115"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="テキスト ボックス 2"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2238375" y="4457700"/>
+              <a:ext cx="395288" cy="279115"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:rad>
+                      <m:radPr>
+                        <m:ctrlPr>
+                          <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:radPr>
+                      <m:deg>
+                        <m:r>
+                          <a:rPr lang="ja-JP" altLang="en-US"/>
+                          <m:t>3</m:t>
+                        </m:r>
+                      </m:deg>
+                      <m:e/>
+                    </m:rad>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="テキスト ボックス 2"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2238375" y="4457700"/>
+              <a:ext cx="395288" cy="279115"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>∛</a:t>
+              </a:r>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>100012</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2045175" cy="223074"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="テキスト ボックス 3"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1471612" y="7253287"/>
+              <a:ext cx="2045175" cy="223074"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑓</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>≔</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−2</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝐵𝑥</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝐶</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=0</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="テキスト ボックス 3"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1471612" y="7253287"/>
+              <a:ext cx="2045175" cy="223074"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑓(𝑥)≔𝑥^2−2𝐵𝑥+𝐶=0</a:t>
               </a:r>
               <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400"/>
             </a:p>
@@ -15471,8 +15863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -15811,19 +16203,19 @@
       </c>
       <c r="E130" s="6">
         <f ca="1">RAND()*10</f>
-        <v>0.69721881222178816</v>
+        <v>1.5613777095521697</v>
       </c>
       <c r="F130" s="6">
         <f ca="1">RAND()*10</f>
-        <v>0.50172406692161164</v>
+        <v>9.1756971777813465</v>
       </c>
       <c r="G130" s="6">
         <f t="array" aca="1" ref="G130:H130" ca="1">TRANSPOSE(MMULT(M_U,TRANSPOSE(E130:F130)))+V_NN</f>
-        <v>-4.8335661631773537</v>
+        <v>3.2514835319954853</v>
       </c>
       <c r="H130" s="6">
         <f ca="1"/>
-        <v>4.6498127984709674</v>
+        <v>7.9081178109488599</v>
       </c>
     </row>
     <row r="131" spans="3:8" x14ac:dyDescent="0.4">
@@ -15833,19 +16225,19 @@
       </c>
       <c r="E131" s="6">
         <f t="shared" ref="E131:F133" ca="1" si="0">RAND()*10</f>
-        <v>8.4663021827176905</v>
+        <v>3.8835988679248867E-2</v>
       </c>
       <c r="F131" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5511220008408637</v>
+        <v>3.9027212035321259</v>
       </c>
       <c r="G131" s="6">
         <f t="array" aca="1" ref="G131:H131" ca="1">TRANSPOSE(MMULT(M_U,TRANSPOSE(E131:F131)))+V_NN</f>
-        <v>-3.1214874903537249</v>
+        <v>-1.3842617214393491</v>
       </c>
       <c r="H131" s="6">
         <f ca="1"/>
-        <v>13.241964255644424</v>
+        <v>4.9700444861210737</v>
       </c>
     </row>
     <row r="132" spans="3:8" x14ac:dyDescent="0.4">
@@ -15855,19 +16247,19 @@
       </c>
       <c r="E132" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.99386746875143706</v>
+        <v>7.9846708039983652</v>
       </c>
       <c r="F132" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>9.5593805909316583</v>
+        <v>2.0550840591688893</v>
       </c>
       <c r="G132" s="6">
         <f t="array" aca="1" ref="G132:H132" ca="1">TRANSPOSE(MMULT(M_U,TRANSPOSE(E132:F132)))+V_NN</f>
-        <v>3.7787224760439893</v>
+        <v>-5.3828271283174089</v>
       </c>
       <c r="H132" s="6">
         <f ca="1"/>
-        <v>7.4707393354622438</v>
+        <v>12.08070750840572</v>
       </c>
     </row>
     <row r="133" spans="3:8" x14ac:dyDescent="0.4">
@@ -15877,19 +16269,19 @@
       </c>
       <c r="E133" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7063501136337305</v>
+        <v>2.7567454201469377</v>
       </c>
       <c r="F133" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>5.8643616804719878</v>
+        <v>0.44260465163959428</v>
       </c>
       <c r="G133" s="6">
         <f t="array" aca="1" ref="G133:H133" ca="1">TRANSPOSE(MMULT(M_U,TRANSPOSE(E133:F133)))+V_NN</f>
-        <v>-1.367990818564337</v>
+        <v>-5.4669882520671322</v>
       </c>
       <c r="H133" s="6">
         <f ca="1"/>
-        <v>11.920117379620537</v>
+        <v>6.6104049058001468</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.4">
@@ -15918,4 +16310,139 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="24.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" ht="19.5" thickTop="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C13" s="21" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C14" s="21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C15" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C16" s="21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C21" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B27" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>